<commit_message>
added rankings + pit scouting information
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="85">
   <si>
     <t>#</t>
   </si>
@@ -115,6 +115,12 @@
     <t>Points</t>
   </si>
   <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
     <t>High</t>
   </si>
   <si>
@@ -148,6 +154,72 @@
     <t>Day 2</t>
   </si>
   <si>
+    <t>Pit Scouting Info</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>email@orangecsd.org</t>
+  </si>
+  <si>
+    <t>Team Number</t>
+  </si>
+  <si>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>Will do right after I finish this form</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>15 m/s</t>
+  </si>
+  <si>
+    <t>Drivetrain</t>
+  </si>
+  <si>
+    <t>Tank</t>
+  </si>
+  <si>
+    <t>Scoring Capabilities</t>
+  </si>
+  <si>
+    <t>Score cones, Score cubes</t>
+  </si>
+  <si>
+    <t>Leave Community?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Starting Position</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>Scoring Method</t>
+  </si>
+  <si>
+    <t>Push with bumpers</t>
+  </si>
+  <si>
+    <t>Defense?</t>
+  </si>
+  <si>
+    <t>Other Information</t>
+  </si>
+  <si>
+    <t>aoecirkra.u89xfa.r9ig.pnuda,oc.ria.pd</t>
+  </si>
+  <si>
     <t>truman</t>
   </si>
   <si>
@@ -157,6 +229,27 @@
     <t>;ekuehiuhehi</t>
   </si>
   <si>
+    <t>test@orangecsd.org</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Swerve</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Shoot at target</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>ben</t>
   </si>
   <si>
@@ -164,6 +257,21 @@
   </si>
   <si>
     <t>ontehu</t>
+  </si>
+  <si>
+    <t>23dsuh@orangecsd.org</t>
+  </si>
+  <si>
+    <t>7 m/s</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Place on target</t>
+  </si>
+  <si>
+    <t>good robot</t>
   </si>
 </sst>
 </file>
@@ -228,19 +336,96 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD580"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD580"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -2981,13 +3166,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3170,19 +3355,62 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:O100">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1787</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E4">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G4">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I4">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K4">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M4">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O4">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BI10"/>
+  <sheetPr>
+    <tabColor rgb="FFFFA500"/>
+  </sheetPr>
+  <dimension ref="A1:BI30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -3246,31 +3474,31 @@
         <v>0</v>
       </c>
       <c r="AZ1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="BA1">
         <v>1</v>
       </c>
       <c r="BB1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="BC1">
         <v>0</v>
       </c>
       <c r="BD1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="BE1">
         <v>0</v>
       </c>
       <c r="BF1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="BG1">
         <v>1</v>
       </c>
       <c r="BH1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="BI1">
         <v>13</v>
@@ -3323,31 +3551,31 @@
         <v>26</v>
       </c>
       <c r="AZ2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="BA2">
         <v>2</v>
       </c>
       <c r="BB2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="BC2">
         <v>0</v>
       </c>
       <c r="BD2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="BE2">
         <v>1</v>
       </c>
       <c r="BF2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="BG2">
         <v>1</v>
       </c>
       <c r="BH2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="BI2">
         <v>0</v>
@@ -3397,25 +3625,25 @@
         <v>30</v>
       </c>
       <c r="AZ3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="BA3">
         <v>0</v>
       </c>
       <c r="BB3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="BC3">
         <v>2</v>
       </c>
       <c r="BD3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="BE3">
         <v>1</v>
       </c>
       <c r="BF3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="BG3">
         <v>0</v>
@@ -3463,44 +3691,184 @@
       </c>
     </row>
     <row r="7" spans="1:61">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:61">
-      <c r="A8">
-        <v>26</v>
+      <c r="A8" t="s">
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="AX8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:61">
-      <c r="A9">
-        <v>-7</v>
+      <c r="A9" t="s">
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:61">
-      <c r="A10">
-        <v>-64</v>
+      <c r="A10" t="s">
+        <v>6</v>
       </c>
       <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:61">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:61">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:61">
+      <c r="A15">
+        <v>26</v>
+      </c>
+      <c r="B15">
         <v>50</v>
       </c>
     </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A18:C18"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A14:C14">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:P1">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3508,13 +3876,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BI10"/>
+  <sheetPr>
+    <tabColor rgb="FFBF6940"/>
+  </sheetPr>
+  <dimension ref="A1:BI30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -3578,31 +3949,31 @@
         <v>135</v>
       </c>
       <c r="AZ1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="BA1">
         <v>22</v>
       </c>
       <c r="BB1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="BC1">
         <v>2</v>
       </c>
       <c r="BD1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="BE1">
         <v>2</v>
       </c>
       <c r="BF1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="BG1">
         <v>0</v>
       </c>
       <c r="BH1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="BI1">
         <v>131.5</v>
@@ -3646,40 +4017,40 @@
         <v>5</v>
       </c>
       <c r="O2" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="P2" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="AY2">
         <v>128</v>
       </c>
       <c r="AZ2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="BA2">
         <v>13</v>
       </c>
       <c r="BB2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="BC2">
         <v>0</v>
       </c>
       <c r="BD2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="BE2">
         <v>0</v>
       </c>
       <c r="BF2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="BG2">
         <v>2</v>
       </c>
       <c r="BH2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="BI2">
         <v>0</v>
@@ -3726,28 +4097,28 @@
         <v>27</v>
       </c>
       <c r="P3" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="AZ3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="BA3">
         <v>8</v>
       </c>
       <c r="BB3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="BC3">
         <v>0</v>
       </c>
       <c r="BD3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="BE3">
         <v>0</v>
       </c>
       <c r="BF3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="BG3">
         <v>0</v>
@@ -3795,44 +4166,184 @@
       </c>
     </row>
     <row r="7" spans="1:61">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:61">
-      <c r="A8">
-        <v>26</v>
+      <c r="A8" t="s">
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="AX8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:61">
-      <c r="A9">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:61">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:61">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:61">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:61">
+      <c r="A15">
         <v>-7</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:61">
-      <c r="A10">
-        <v>-64</v>
-      </c>
-      <c r="B10">
-        <v>50</v>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A18:C18"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A14:C14">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:P1">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3840,13 +4351,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BI10"/>
+  <sheetPr>
+    <tabColor rgb="FF808080"/>
+  </sheetPr>
+  <dimension ref="A1:BI30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -3910,31 +4424,31 @@
         <v>77</v>
       </c>
       <c r="AZ1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="BA1">
         <v>10</v>
       </c>
       <c r="BB1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="BC1">
         <v>1</v>
       </c>
       <c r="BD1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="BE1">
         <v>1</v>
       </c>
       <c r="BF1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="BG1">
         <v>1</v>
       </c>
       <c r="BH1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="BI1">
         <v>45</v>
@@ -3981,37 +4495,37 @@
         <v>27</v>
       </c>
       <c r="P2" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="AY2">
         <v>13</v>
       </c>
       <c r="AZ2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="BA2">
         <v>0</v>
       </c>
       <c r="BB2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="BC2">
         <v>0</v>
       </c>
       <c r="BD2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="BE2">
         <v>0</v>
       </c>
       <c r="BF2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="BG2">
         <v>1</v>
       </c>
       <c r="BH2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="BI2">
         <v>0</v>
@@ -4055,31 +4569,31 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="P3" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="AZ3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="BA3">
         <v>0</v>
       </c>
       <c r="BB3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="BC3">
         <v>1</v>
       </c>
       <c r="BD3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="BE3">
         <v>1</v>
       </c>
       <c r="BF3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="BG3">
         <v>0</v>
@@ -4127,44 +4641,184 @@
       </c>
     </row>
     <row r="7" spans="1:61">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:61">
-      <c r="A8">
-        <v>26</v>
+      <c r="A8" t="s">
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="AX8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:61">
-      <c r="A9">
-        <v>-7</v>
+      <c r="A9" t="s">
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:61">
-      <c r="A10">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:61">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:61">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:61">
+      <c r="A15">
         <v>-64</v>
       </c>
-      <c r="B10">
+      <c r="B15">
         <v>50</v>
       </c>
     </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A18:C18"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A14:C14">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:P1">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>-99999999999</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>